<commit_message>
Added total cost to the sheet
</commit_message>
<xml_diff>
--- a/ProjectProp.xlsx
+++ b/ProjectProp.xlsx
@@ -5,7 +5,7 @@
   <workbookPr checkCompatibility="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steffen/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steffen/GitHub/SPARC-Auburn/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Project Idea</t>
   </si>
@@ -33,6 +33,9 @@
   </si>
   <si>
     <t>Cost</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -160,18 +163,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -179,10 +170,22 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -531,7 +534,7 @@
   <dimension ref="A1:L29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -540,199 +543,207 @@
     <col min="2" max="2" width="14.83203125" customWidth="1"/>
     <col min="6" max="6" width="27.5" style="1" customWidth="1"/>
     <col min="7" max="7" width="13.6640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="16" customWidth="1"/>
+    <col min="12" max="12" width="24.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="10" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
+      <c r="H1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="L1" s="12"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="H2">
+        <f>SUM(G2:G30)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
+      <c r="A3" s="11"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="F4" s="9"/>
+      <c r="A4" s="11"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="F4" s="5"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
+      <c r="A5" s="11"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
+      <c r="A6" s="11"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="F7" s="9"/>
+      <c r="A7" s="11"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="F7" s="5"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
+      <c r="A8" s="11"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
+      <c r="A9" s="11"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+    </row>
+    <row r="10" spans="1:12" ht="21" x14ac:dyDescent="0.25">
+      <c r="A10" s="11"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="L10" s="12"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
+      <c r="A11" s="11"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
+      <c r="A12" s="11"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
       <c r="E12" s="3"/>
       <c r="H12" s="2"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
+      <c r="A13" s="11"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
+      <c r="A14" s="11"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
+      <c r="A15" s="11"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
+      <c r="A16" s="11"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
+      <c r="A17" s="11"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
+      <c r="A18" s="11"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
+      <c r="A19" s="11"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
+      <c r="A20" s="11"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
+      <c r="A21" s="11"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="4"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
+      <c r="A22" s="11"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="4"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
+      <c r="A23" s="11"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="4"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
+      <c r="A24" s="11"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="4"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
+      <c r="A25" s="11"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="4"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
+      <c r="A26" s="11"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="4"/>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
+      <c r="A27" s="11"/>
+      <c r="B27" s="11"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="11"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="4"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
+      <c r="A28" s="11"/>
+      <c r="B28" s="11"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="4"/>
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
+      <c r="A29" s="11"/>
+      <c r="B29" s="11"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>